<commit_message>
Adding the Shortcut-Hotkey Extension
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/PM-Sheet.xlsx
+++ b/01_ProjectPlanning/PM-Sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\Neuer Ordner\ProjectPlanning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\WinAutomatedSimplifier\WinAutomatedSimplifier\01_ProjectPlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Task</t>
   </si>
@@ -72,6 +72,15 @@
   </si>
   <si>
     <t>1. Woche</t>
+  </si>
+  <si>
+    <t>2. Woche</t>
+  </si>
+  <si>
+    <t>ShortcutDialog</t>
+  </si>
+  <si>
+    <t>Folder-Observer</t>
   </si>
 </sst>
 </file>
@@ -131,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -157,6 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -477,11 +487,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -514,14 +524,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -554,7 +564,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E9" si="0">IF(C4="",B4,C4) - D4</f>
+        <f t="shared" ref="E4:E12" si="0">IF(C4="",B4,C4) - D4</f>
         <v>0</v>
       </c>
       <c r="F4" s="6" t="s">
@@ -660,14 +670,82 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="A10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.13541666666666666</v>
+      </c>
+      <c r="D11" s="11">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E11" s="1">
+        <f>IF(C11="",B11,C11) - D11</f>
+        <v>0.12847222222222221</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <f>IF(C12="",B12,C12) - D12</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="5:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="5:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="5:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="5:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="5:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>